<commit_message>
Thu Feb  6 06:50:05 AM CST 2025
</commit_message>
<xml_diff>
--- a/bosai/summary/assess.xlsx
+++ b/bosai/summary/assess.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11355" tabRatio="748" activeTab="3"/>
+    <workbookView windowWidth="28800" windowHeight="11355" tabRatio="748" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="第一个月产出汇总" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="199">
   <si>
     <t>试用期项目完成情况汇总表（第一个月）</t>
   </si>
@@ -799,6 +799,30 @@
       </rPr>
       <t xml:space="preserve">    </t>
     </r>
+  </si>
+  <si>
+    <t>BSJF240734, 清心莲子饮补充分子对接</t>
+  </si>
+  <si>
+    <t>BSYB250111, 骨质疏松</t>
+  </si>
+  <si>
+    <t>BS.asis, 子宫内膜异位</t>
+  </si>
+  <si>
+    <t>BSCL241113, 再生障碍贫血</t>
+  </si>
+  <si>
+    <t>还未上传</t>
+  </si>
+  <si>
+    <t>BS.develop, scFEA 用于单细胞数据预测代谢通量配置与调试</t>
+  </si>
+  <si>
+    <t>BS.develop, TWAS 相关程序配置与调试</t>
+  </si>
+  <si>
+    <t>BSDG250121, 哮喘相关</t>
   </si>
   <si>
     <r>
@@ -1530,16 +1554,20 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="仿宋"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <sz val="12"/>
+      <name val="仿宋"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="仿宋"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1562,20 +1590,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="仿宋"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="仿宋"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="仿宋"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -4111,7 +4135,7 @@
   <sheetPr/>
   <dimension ref="B1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -4480,8 +4504,8 @@
   <sheetPr/>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" outlineLevelCol="5"/>
@@ -4875,10 +4899,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:H18"/>
+  <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.9" customHeight="1" outlineLevelCol="7"/>
@@ -5039,82 +5063,174 @@
       </c>
     </row>
     <row r="11" customHeight="1" spans="2:8">
-      <c r="B11" s="92"/>
-      <c r="C11" s="98"/>
-      <c r="D11" s="92"/>
+      <c r="B11" s="92" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="98" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="92">
+        <v>2</v>
+      </c>
       <c r="E11" s="95"/>
       <c r="F11" s="115"/>
       <c r="G11" s="116"/>
       <c r="H11" s="92"/>
     </row>
     <row r="12" customHeight="1" spans="2:8">
-      <c r="B12" s="92"/>
-      <c r="C12" s="98"/>
-      <c r="D12" s="92"/>
+      <c r="B12" s="92" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="98" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="92">
+        <v>8</v>
+      </c>
       <c r="E12" s="95"/>
       <c r="F12" s="115"/>
       <c r="G12" s="116"/>
       <c r="H12" s="92"/>
     </row>
     <row r="13" customHeight="1" spans="2:8">
-      <c r="B13" s="92"/>
-      <c r="C13" s="98"/>
-      <c r="D13" s="92"/>
+      <c r="B13" s="92" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="98" t="s">
+        <v>105</v>
+      </c>
+      <c r="D13" s="92">
+        <v>8</v>
+      </c>
       <c r="E13" s="95"/>
       <c r="F13" s="115"/>
       <c r="G13" s="117"/>
       <c r="H13" s="92"/>
     </row>
     <row r="14" customHeight="1" spans="2:8">
-      <c r="B14" s="92"/>
-      <c r="C14" s="98"/>
-      <c r="D14" s="92"/>
+      <c r="B14" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="98" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="92">
+        <v>3</v>
+      </c>
       <c r="E14" s="92"/>
       <c r="F14" s="115"/>
       <c r="G14" s="117"/>
       <c r="H14" s="92"/>
     </row>
     <row r="15" customHeight="1" spans="2:8">
-      <c r="B15" s="92"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="92"/>
-      <c r="E15" s="95"/>
+      <c r="B15" s="92" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="98" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="92">
+        <v>2</v>
+      </c>
+      <c r="E15" s="92"/>
       <c r="F15" s="115"/>
       <c r="G15" s="117"/>
       <c r="H15" s="92"/>
     </row>
     <row r="16" customHeight="1" spans="2:8">
-      <c r="B16" s="92"/>
-      <c r="C16" s="92" t="s">
+      <c r="B16" s="92" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="98" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="92">
+        <v>20</v>
+      </c>
+      <c r="E16" s="92"/>
+      <c r="F16" s="115"/>
+      <c r="G16" s="117"/>
+      <c r="H16" s="92" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" spans="2:8">
+      <c r="B17" s="92" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="98" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="92">
+        <v>20</v>
+      </c>
+      <c r="E17" s="92"/>
+      <c r="F17" s="115"/>
+      <c r="G17" s="117"/>
+      <c r="H17" s="92"/>
+    </row>
+    <row r="18" customHeight="1" spans="2:8">
+      <c r="B18" s="92" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="98" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="92">
+        <v>20</v>
+      </c>
+      <c r="E18" s="92"/>
+      <c r="F18" s="115"/>
+      <c r="G18" s="117"/>
+      <c r="H18" s="92"/>
+    </row>
+    <row r="19" customHeight="1" spans="2:8">
+      <c r="B19" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="98" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" s="92">
+        <v>3</v>
+      </c>
+      <c r="E19" s="95"/>
+      <c r="F19" s="115"/>
+      <c r="G19" s="117"/>
+      <c r="H19" s="92"/>
+    </row>
+    <row r="20" customHeight="1" spans="2:8">
+      <c r="B20" s="92"/>
+      <c r="C20" s="92" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="92"/>
-      <c r="E16" s="95"/>
-      <c r="F16" s="115"/>
-      <c r="G16" s="116"/>
-      <c r="H16" s="92"/>
-    </row>
-    <row r="17" ht="79.05" customHeight="1" spans="2:8">
-      <c r="B17" s="99" t="s">
-        <v>111</v>
-      </c>
-      <c r="C17" s="100"/>
-      <c r="D17" s="100"/>
-      <c r="E17" s="100"/>
-      <c r="F17" s="100"/>
-      <c r="G17" s="100"/>
-      <c r="H17" s="118"/>
-    </row>
-    <row r="18" ht="136.5" customHeight="1" spans="2:8">
-      <c r="B18" s="101" t="s">
+      <c r="D20" s="92"/>
+      <c r="E20" s="95"/>
+      <c r="F20" s="115"/>
+      <c r="G20" s="116"/>
+      <c r="H20" s="92"/>
+    </row>
+    <row r="21" ht="79.05" customHeight="1" spans="2:8">
+      <c r="B21" s="99" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" s="100"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="100"/>
+      <c r="F21" s="100"/>
+      <c r="G21" s="100"/>
+      <c r="H21" s="118"/>
+    </row>
+    <row r="22" ht="136.5" customHeight="1" spans="2:8">
+      <c r="B22" s="101" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="102"/>
-      <c r="D18" s="102"/>
-      <c r="E18" s="102"/>
-      <c r="F18" s="102"/>
-      <c r="G18" s="102"/>
-      <c r="H18" s="119"/>
+      <c r="C22" s="102"/>
+      <c r="D22" s="102"/>
+      <c r="E22" s="102"/>
+      <c r="F22" s="102"/>
+      <c r="G22" s="102"/>
+      <c r="H22" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -5127,10 +5243,10 @@
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B22:H22"/>
     <mergeCell ref="H4:H8"/>
     <mergeCell ref="F4:G8"/>
   </mergeCells>
@@ -5148,7 +5264,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15:F18"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" outlineLevelCol="5"/>
@@ -5165,7 +5281,7 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:6">
       <c r="A1" s="59" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
@@ -5184,7 +5300,7 @@
         <v>46</v>
       </c>
       <c r="D2" s="62" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="E2" s="61" t="s">
         <v>48</v>
@@ -5198,7 +5314,7 @@
         <v>50</v>
       </c>
       <c r="B3" s="64" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="C3" s="65"/>
       <c r="D3" s="65"/>
@@ -5233,7 +5349,9 @@
       </c>
       <c r="D5" s="62"/>
       <c r="E5" s="62"/>
-      <c r="F5" s="83"/>
+      <c r="F5" s="83">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">
       <c r="A6" s="70"/>
@@ -5267,7 +5385,9 @@
       </c>
       <c r="D8" s="65"/>
       <c r="E8" s="81"/>
-      <c r="F8" s="83"/>
+      <c r="F8" s="83">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" customHeight="1" spans="1:6">
       <c r="A9" s="75"/>
@@ -5311,7 +5431,9 @@
       </c>
       <c r="D12" s="62"/>
       <c r="E12" s="62"/>
-      <c r="F12" s="83"/>
+      <c r="F12" s="83">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" customHeight="1" spans="1:6">
       <c r="A13" s="75"/>
@@ -5345,7 +5467,9 @@
       </c>
       <c r="D15" s="65"/>
       <c r="E15" s="81"/>
-      <c r="F15" s="83"/>
+      <c r="F15" s="83">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" customHeight="1" spans="1:6">
       <c r="A16" s="75"/>
@@ -5389,7 +5513,9 @@
       </c>
       <c r="D19" s="65"/>
       <c r="E19" s="81"/>
-      <c r="F19" s="83"/>
+      <c r="F19" s="83">
+        <v>17</v>
+      </c>
     </row>
     <row r="20" customHeight="1" spans="1:6">
       <c r="A20" s="75"/>
@@ -5433,7 +5559,9 @@
       </c>
       <c r="D23" s="65"/>
       <c r="E23" s="81"/>
-      <c r="F23" s="83"/>
+      <c r="F23" s="83">
+        <v>13</v>
+      </c>
     </row>
     <row r="24" customHeight="1" spans="1:6">
       <c r="A24" s="75"/>
@@ -5477,7 +5605,7 @@
     </row>
     <row r="29" customHeight="1" spans="1:1">
       <c r="A29" s="55" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -5560,7 +5688,7 @@
   <sheetData>
     <row r="1" ht="47.1" customHeight="1" spans="1:10">
       <c r="A1" s="23" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -5574,39 +5702,39 @@
     </row>
     <row r="2" ht="29.1" customHeight="1" spans="1:10">
       <c r="A2" s="24" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
       <c r="D2" s="25"/>
       <c r="E2" s="25" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="H2" s="25"/>
       <c r="I2" s="25" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="J2" s="45"/>
     </row>
     <row r="3" ht="27" customHeight="1" spans="1:10">
       <c r="A3" s="26" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
       <c r="D3" s="27"/>
       <c r="E3" s="27" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="F3" s="27"/>
       <c r="G3" s="27" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="H3" s="27"/>
       <c r="I3" s="46"/>
@@ -5614,7 +5742,7 @@
     </row>
     <row r="4" ht="14.25" customHeight="1" spans="1:10">
       <c r="A4" s="28" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
@@ -5628,11 +5756,11 @@
     </row>
     <row r="5" ht="14.25" customHeight="1" spans="1:10">
       <c r="A5" s="29" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="30" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="D5" s="31"/>
       <c r="E5" s="31"/>
@@ -5658,7 +5786,7 @@
       <c r="A7" s="29"/>
       <c r="B7" s="29"/>
       <c r="C7" s="30" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="D7" s="31"/>
       <c r="E7" s="31"/>
@@ -5682,11 +5810,11 @@
     </row>
     <row r="9" ht="14.25" customHeight="1" spans="1:10">
       <c r="A9" s="36" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B9" s="36"/>
       <c r="C9" s="30" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="31"/>
@@ -5712,7 +5840,7 @@
       <c r="A11" s="36"/>
       <c r="B11" s="36"/>
       <c r="C11" s="37" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="D11" s="38"/>
       <c r="E11" s="38"/>
@@ -5738,7 +5866,7 @@
       <c r="A13" s="36"/>
       <c r="B13" s="36"/>
       <c r="C13" s="37" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="D13" s="38"/>
       <c r="E13" s="38"/>
@@ -5762,11 +5890,11 @@
     </row>
     <row r="15" ht="14.25" customHeight="1" spans="1:10">
       <c r="A15" s="36" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B15" s="36"/>
       <c r="C15" s="37" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="D15" s="38"/>
       <c r="E15" s="38"/>
@@ -5792,7 +5920,7 @@
       <c r="A17" s="36"/>
       <c r="B17" s="36"/>
       <c r="C17" s="37" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="D17" s="38"/>
       <c r="E17" s="38"/>
@@ -5816,11 +5944,11 @@
     </row>
     <row r="19" ht="14.25" customHeight="1" spans="1:10">
       <c r="A19" s="36" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="B19" s="36"/>
       <c r="C19" s="37" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="D19" s="38"/>
       <c r="E19" s="38"/>
@@ -5846,7 +5974,7 @@
       <c r="A21" s="36"/>
       <c r="B21" s="36"/>
       <c r="C21" s="37" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="D21" s="38"/>
       <c r="E21" s="38"/>
@@ -5870,7 +5998,7 @@
     </row>
     <row r="23" ht="14.25" customHeight="1" spans="1:10">
       <c r="A23" s="41" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="B23" s="41"/>
       <c r="C23" s="41"/>
@@ -5884,10 +6012,10 @@
     </row>
     <row r="24" ht="14.25" customHeight="1" spans="1:10">
       <c r="A24" s="36" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="C24" s="38"/>
       <c r="D24" s="38"/>
@@ -5912,10 +6040,10 @@
     </row>
     <row r="26" ht="14.25" customHeight="1" spans="1:10">
       <c r="A26" s="36" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="C26" s="38"/>
       <c r="D26" s="38"/>
@@ -5940,10 +6068,10 @@
     </row>
     <row r="28" ht="14.25" customHeight="1" spans="1:10">
       <c r="A28" s="36" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="C28" s="38"/>
       <c r="D28" s="38"/>
@@ -5968,10 +6096,10 @@
     </row>
     <row r="30" ht="14.25" customHeight="1" spans="1:10">
       <c r="A30" s="44" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="C30" s="38"/>
       <c r="D30" s="38"/>
@@ -6063,36 +6191,36 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:5">
@@ -6119,13 +6247,13 @@
     <row r="6" ht="75" customHeight="1" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="8" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="E6" s="17"/>
     </row>
@@ -6135,13 +6263,13 @@
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:5">
@@ -6149,78 +6277,78 @@
         <v>20</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:5">
       <c r="A9" s="12"/>
       <c r="B9" s="8" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="E9" s="20"/>
     </row>
     <row r="10" customHeight="1" spans="1:5">
       <c r="A10" s="12"/>
       <c r="B10" s="8" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="E10" s="20"/>
     </row>
     <row r="11" ht="60" customHeight="1" spans="1:5">
       <c r="A11" s="13"/>
       <c r="B11" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>164</v>
-      </c>
       <c r="D11" s="8" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="E11" s="21"/>
     </row>
     <row r="12" customHeight="1" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:5">
       <c r="A13" s="1"/>
       <c r="B13" s="8" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -6229,7 +6357,7 @@
     <row r="14" ht="11" customHeight="1" spans="1:5">
       <c r="A14" s="1"/>
       <c r="B14" s="8" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -6237,72 +6365,72 @@
     </row>
     <row r="15" customHeight="1" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" ht="66" customHeight="1" spans="1:5">
       <c r="A16" s="1"/>
       <c r="B16" s="8" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="E16" s="17"/>
     </row>
     <row r="17" customHeight="1" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="E17" s="8"/>
     </row>
     <row r="18" customHeight="1" spans="1:5">
       <c r="A18" s="1"/>
       <c r="B18" s="8" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="E18" s="8"/>
     </row>
     <row r="19" ht="60" customHeight="1" spans="1:5">
       <c r="A19" s="1"/>
       <c r="B19" s="8" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="E19" s="8"/>
     </row>
     <row r="20" ht="261" customHeight="1" spans="1:5">
       <c r="A20" s="14" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -6311,7 +6439,7 @@
     </row>
     <row r="22" ht="39" customHeight="1" spans="1:1">
       <c r="A22" s="16" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fri Feb  7 06:50:05 AM CST 2025
</commit_message>
<xml_diff>
--- a/bosai/summary/assess.xlsx
+++ b/bosai/summary/assess.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11355" tabRatio="748" activeTab="4"/>
+    <workbookView windowWidth="28800" windowHeight="11355" tabRatio="748"/>
   </bookViews>
   <sheets>
     <sheet name="第一个月产出汇总" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="200">
   <si>
     <t>试用期项目完成情况汇总表（第一个月）</t>
   </si>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t>BSHQ240303, ZDHHC15互作蛋白筛选</t>
+  </si>
+  <si>
+    <t>BSZD231122杨立宇(完成20%）</t>
   </si>
   <si>
     <t>合计</t>
@@ -1272,7 +1275,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="48">
+  <fonts count="49">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1373,6 +1376,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1554,23 +1563,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="仿宋"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="仿宋"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="仿宋"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <name val="宋体"/>
@@ -1590,15 +1582,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="仿宋"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="仿宋"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="仿宋"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -1809,7 +1818,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -2181,6 +2190,21 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2300,137 +2324,137 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2772,6 +2796,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2793,43 +2820,43 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3298,8 +3325,8 @@
   </sheetPr>
   <dimension ref="B1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.9" customHeight="1"/>
@@ -3316,16 +3343,16 @@
   </cols>
   <sheetData>
     <row r="1" ht="45" customHeight="1" spans="2:9">
-      <c r="B1" s="123" t="s">
+      <c r="B1" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="134"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="135"/>
     </row>
     <row r="2" ht="45" customHeight="1" spans="2:9">
       <c r="B2" s="89" t="s">
@@ -3337,118 +3364,118 @@
       <c r="F2" s="89"/>
       <c r="G2" s="89"/>
       <c r="H2" s="89"/>
-      <c r="I2" s="134"/>
+      <c r="I2" s="135"/>
     </row>
     <row r="3" ht="34.95" customHeight="1" spans="2:9">
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="124" t="s">
+      <c r="C3" s="125" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="124" t="s">
+      <c r="D3" s="125" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="124" t="s">
+      <c r="E3" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="129" t="s">
+      <c r="F3" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="130"/>
-      <c r="H3" s="124" t="s">
+      <c r="G3" s="131"/>
+      <c r="H3" s="125" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="134"/>
+      <c r="I3" s="135"/>
     </row>
     <row r="4" ht="34.95" customHeight="1" spans="2:9">
-      <c r="B4" s="125" t="s">
+      <c r="B4" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="125" t="s">
+      <c r="C4" s="126" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="125" t="s">
+      <c r="D4" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="125" t="s">
+      <c r="E4" s="126" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="105" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="106"/>
-      <c r="H4" s="131" t="s">
+      <c r="H4" s="132" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="134"/>
+      <c r="I4" s="135"/>
     </row>
     <row r="5" ht="100.05" customHeight="1" spans="2:9">
-      <c r="B5" s="126" t="s">
+      <c r="B5" s="127" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="127" t="s">
+      <c r="C5" s="128" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="126"/>
-      <c r="E5" s="126"/>
+      <c r="D5" s="127"/>
+      <c r="E5" s="127"/>
       <c r="F5" s="108"/>
       <c r="G5" s="109"/>
-      <c r="H5" s="132"/>
-      <c r="I5" s="134"/>
+      <c r="H5" s="133"/>
+      <c r="I5" s="135"/>
     </row>
     <row r="6" ht="100.05" customHeight="1" spans="2:9">
-      <c r="B6" s="126" t="s">
+      <c r="B6" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="127" t="s">
+      <c r="C6" s="128" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="126"/>
-      <c r="E6" s="126"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
       <c r="F6" s="108"/>
       <c r="G6" s="109"/>
-      <c r="H6" s="132"/>
-      <c r="I6" s="134"/>
+      <c r="H6" s="133"/>
+      <c r="I6" s="135"/>
     </row>
     <row r="7" ht="100.05" customHeight="1" spans="2:9">
-      <c r="B7" s="126" t="s">
+      <c r="B7" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="127" t="s">
+      <c r="C7" s="128" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="126"/>
-      <c r="E7" s="126"/>
+      <c r="D7" s="127"/>
+      <c r="E7" s="127"/>
       <c r="F7" s="108"/>
       <c r="G7" s="109"/>
-      <c r="H7" s="132"/>
-      <c r="I7" s="134"/>
+      <c r="H7" s="133"/>
+      <c r="I7" s="135"/>
     </row>
     <row r="8" ht="100.05" customHeight="1" spans="2:9">
-      <c r="B8" s="126" t="s">
+      <c r="B8" s="127" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="127" t="s">
+      <c r="C8" s="128" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="126"/>
-      <c r="E8" s="126"/>
+      <c r="D8" s="127"/>
+      <c r="E8" s="127"/>
       <c r="F8" s="111"/>
       <c r="G8" s="112"/>
-      <c r="H8" s="133"/>
-      <c r="I8" s="134"/>
+      <c r="H8" s="134"/>
+      <c r="I8" s="135"/>
     </row>
     <row r="9" customHeight="1" spans="2:8">
-      <c r="B9" s="128" t="s">
+      <c r="B9" s="129" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="128"/>
-      <c r="D9" s="128"/>
-      <c r="E9" s="128"/>
-      <c r="F9" s="128"/>
-      <c r="G9" s="128"/>
-      <c r="H9" s="128"/>
+      <c r="C9" s="129"/>
+      <c r="D9" s="129"/>
+      <c r="E9" s="129"/>
+      <c r="F9" s="129"/>
+      <c r="G9" s="129"/>
+      <c r="H9" s="129"/>
     </row>
     <row r="10" ht="42.9" customHeight="1" spans="2:9">
       <c r="B10" s="91" t="s">
@@ -3484,9 +3511,11 @@
       <c r="D11" s="92">
         <v>3</v>
       </c>
-      <c r="E11" s="95"/>
-      <c r="F11" s="115"/>
-      <c r="G11" s="116"/>
+      <c r="E11" s="115">
+        <v>6</v>
+      </c>
+      <c r="F11" s="116"/>
+      <c r="G11" s="117"/>
       <c r="H11" s="92"/>
     </row>
     <row r="12" customHeight="1" spans="2:8">
@@ -3499,9 +3528,11 @@
       <c r="D12" s="92">
         <v>3</v>
       </c>
-      <c r="E12" s="92"/>
-      <c r="F12" s="115"/>
-      <c r="G12" s="116"/>
+      <c r="E12" s="115">
+        <v>6</v>
+      </c>
+      <c r="F12" s="116"/>
+      <c r="G12" s="117"/>
       <c r="H12" s="92"/>
     </row>
     <row r="13" customHeight="1" spans="2:9">
@@ -3512,9 +3543,11 @@
         <v>31</v>
       </c>
       <c r="D13" s="92"/>
-      <c r="E13" s="95"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="117"/>
+      <c r="E13" s="115">
+        <v>20</v>
+      </c>
+      <c r="F13" s="116"/>
+      <c r="G13" s="118"/>
       <c r="H13" s="92"/>
       <c r="I13" s="22" t="s">
         <v>32</v>
@@ -3530,9 +3563,11 @@
       <c r="D14" s="92">
         <v>3</v>
       </c>
-      <c r="E14" s="95"/>
-      <c r="F14" s="115"/>
-      <c r="G14" s="117"/>
+      <c r="E14" s="115">
+        <v>6</v>
+      </c>
+      <c r="F14" s="116"/>
+      <c r="G14" s="118"/>
       <c r="H14" s="92"/>
     </row>
     <row r="15" customHeight="1" spans="2:8">
@@ -3543,9 +3578,11 @@
         <v>34</v>
       </c>
       <c r="D15" s="92"/>
-      <c r="E15" s="95"/>
-      <c r="F15" s="115"/>
-      <c r="G15" s="117"/>
+      <c r="E15" s="115">
+        <v>10</v>
+      </c>
+      <c r="F15" s="116"/>
+      <c r="G15" s="118"/>
       <c r="H15" s="92"/>
     </row>
     <row r="16" customHeight="1" spans="2:8">
@@ -3558,9 +3595,11 @@
       <c r="D16" s="92">
         <v>3</v>
       </c>
-      <c r="E16" s="92"/>
-      <c r="F16" s="115"/>
-      <c r="G16" s="117"/>
+      <c r="E16" s="115">
+        <v>6</v>
+      </c>
+      <c r="F16" s="116"/>
+      <c r="G16" s="118"/>
       <c r="H16" s="92"/>
     </row>
     <row r="17" customHeight="1" spans="2:8">
@@ -3571,9 +3610,11 @@
         <v>37</v>
       </c>
       <c r="D17" s="92"/>
-      <c r="E17" s="92"/>
-      <c r="F17" s="115"/>
-      <c r="G17" s="117"/>
+      <c r="E17" s="115">
+        <v>10</v>
+      </c>
+      <c r="F17" s="116"/>
+      <c r="G17" s="118"/>
       <c r="H17" s="92"/>
     </row>
     <row r="18" customHeight="1" spans="2:8">
@@ -3584,9 +3625,11 @@
         <v>38</v>
       </c>
       <c r="D18" s="92"/>
-      <c r="E18" s="95"/>
-      <c r="F18" s="115"/>
-      <c r="G18" s="117"/>
+      <c r="E18" s="115">
+        <v>6</v>
+      </c>
+      <c r="F18" s="116"/>
+      <c r="G18" s="118"/>
       <c r="H18" s="92"/>
     </row>
     <row r="19" customHeight="1" spans="2:8">
@@ -3597,18 +3640,26 @@
         <v>39</v>
       </c>
       <c r="D19" s="92"/>
-      <c r="E19" s="95"/>
-      <c r="F19" s="115"/>
-      <c r="G19" s="116"/>
+      <c r="E19" s="115">
+        <v>4</v>
+      </c>
+      <c r="F19" s="116"/>
+      <c r="G19" s="117"/>
       <c r="H19" s="92"/>
     </row>
     <row r="20" customHeight="1" spans="2:8">
-      <c r="B20" s="92"/>
-      <c r="C20" s="92"/>
+      <c r="B20" s="115" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="115" t="s">
+        <v>40</v>
+      </c>
       <c r="D20" s="92"/>
-      <c r="E20" s="92"/>
-      <c r="F20" s="115"/>
-      <c r="G20" s="116"/>
+      <c r="E20" s="115">
+        <v>5</v>
+      </c>
+      <c r="F20" s="116"/>
+      <c r="G20" s="117"/>
       <c r="H20" s="92"/>
     </row>
     <row r="21" customHeight="1" spans="2:8">
@@ -3616,8 +3667,8 @@
       <c r="C21" s="92"/>
       <c r="D21" s="92"/>
       <c r="E21" s="95"/>
-      <c r="F21" s="115"/>
-      <c r="G21" s="116"/>
+      <c r="F21" s="116"/>
+      <c r="G21" s="117"/>
       <c r="H21" s="92"/>
     </row>
     <row r="22" customHeight="1" spans="2:8">
@@ -3625,8 +3676,8 @@
       <c r="C22" s="92"/>
       <c r="D22" s="92"/>
       <c r="E22" s="95"/>
-      <c r="F22" s="115"/>
-      <c r="G22" s="116"/>
+      <c r="F22" s="116"/>
+      <c r="G22" s="117"/>
       <c r="H22" s="92"/>
     </row>
     <row r="23" customHeight="1" spans="2:8">
@@ -3634,8 +3685,8 @@
       <c r="C23" s="92"/>
       <c r="D23" s="92"/>
       <c r="E23" s="95"/>
-      <c r="F23" s="115"/>
-      <c r="G23" s="116"/>
+      <c r="F23" s="116"/>
+      <c r="G23" s="117"/>
       <c r="H23" s="92"/>
     </row>
     <row r="24" customHeight="1" spans="2:8">
@@ -3643,8 +3694,8 @@
       <c r="C24" s="92"/>
       <c r="D24" s="92"/>
       <c r="E24" s="92"/>
-      <c r="F24" s="115"/>
-      <c r="G24" s="116"/>
+      <c r="F24" s="116"/>
+      <c r="G24" s="117"/>
       <c r="H24" s="92"/>
     </row>
     <row r="25" customHeight="1" spans="2:8">
@@ -3652,8 +3703,8 @@
       <c r="C25" s="92"/>
       <c r="D25" s="92"/>
       <c r="E25" s="92"/>
-      <c r="F25" s="115"/>
-      <c r="G25" s="116"/>
+      <c r="F25" s="116"/>
+      <c r="G25" s="117"/>
       <c r="H25" s="92"/>
     </row>
     <row r="26" customHeight="1" spans="2:8">
@@ -3661,8 +3712,8 @@
       <c r="C26" s="92"/>
       <c r="D26" s="92"/>
       <c r="E26" s="95"/>
-      <c r="F26" s="115"/>
-      <c r="G26" s="116"/>
+      <c r="F26" s="116"/>
+      <c r="G26" s="117"/>
       <c r="H26" s="92"/>
     </row>
     <row r="27" customHeight="1" spans="2:8">
@@ -3670,42 +3721,45 @@
       <c r="C27" s="92"/>
       <c r="D27" s="92"/>
       <c r="E27" s="95"/>
-      <c r="F27" s="115"/>
-      <c r="G27" s="116"/>
+      <c r="F27" s="116"/>
+      <c r="G27" s="117"/>
       <c r="H27" s="92"/>
     </row>
     <row r="28" customHeight="1" spans="2:8">
       <c r="B28" s="92"/>
       <c r="C28" s="92" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D28" s="92"/>
-      <c r="E28" s="95"/>
-      <c r="F28" s="115"/>
-      <c r="G28" s="116"/>
+      <c r="E28" s="95">
+        <f>SUM(E11:E20)</f>
+        <v>79</v>
+      </c>
+      <c r="F28" s="116"/>
+      <c r="G28" s="117"/>
       <c r="H28" s="92"/>
     </row>
     <row r="29" ht="91.95" customHeight="1" spans="2:8">
       <c r="B29" s="99" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C29" s="100"/>
       <c r="D29" s="100"/>
       <c r="E29" s="100"/>
       <c r="F29" s="100"/>
       <c r="G29" s="100"/>
-      <c r="H29" s="118"/>
+      <c r="H29" s="119"/>
     </row>
     <row r="30" ht="150" customHeight="1" spans="2:8">
       <c r="B30" s="101" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C30" s="102"/>
       <c r="D30" s="102"/>
       <c r="E30" s="102"/>
       <c r="F30" s="102"/>
       <c r="G30" s="102"/>
-      <c r="H30" s="119"/>
+      <c r="H30" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -3754,7 +3808,7 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:6">
       <c r="A1" s="59" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
@@ -3764,30 +3818,30 @@
     </row>
     <row r="2" customHeight="1" spans="1:6">
       <c r="A2" s="61" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" s="62" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" s="63" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" s="62" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" s="61" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F2" s="80" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:6">
       <c r="A3" s="61" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B3" s="64" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C3" s="65"/>
       <c r="D3" s="65"/>
@@ -3796,29 +3850,29 @@
     </row>
     <row r="4" s="55" customFormat="1" customHeight="1" spans="1:6">
       <c r="A4" s="61" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" s="63" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C4" s="66" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D4" s="67"/>
       <c r="E4" s="82"/>
       <c r="F4" s="61" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="68" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B5" s="69" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D5" s="62"/>
       <c r="E5" s="62"/>
@@ -3830,7 +3884,7 @@
       <c r="A6" s="70"/>
       <c r="B6" s="71"/>
       <c r="C6" s="62" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D6" s="62"/>
       <c r="E6" s="62"/>
@@ -3840,7 +3894,7 @@
       <c r="A7" s="72"/>
       <c r="B7" s="73"/>
       <c r="C7" s="62" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D7" s="62"/>
       <c r="E7" s="62"/>
@@ -3848,13 +3902,13 @@
     </row>
     <row r="8" customHeight="1" spans="1:6">
       <c r="A8" s="74" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B8" s="69" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C8" s="64" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D8" s="65"/>
       <c r="E8" s="81"/>
@@ -3866,7 +3920,7 @@
       <c r="A9" s="75"/>
       <c r="B9" s="71"/>
       <c r="C9" s="64" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D9" s="65"/>
       <c r="E9" s="81"/>
@@ -3876,7 +3930,7 @@
       <c r="A10" s="75"/>
       <c r="B10" s="71"/>
       <c r="C10" s="64" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D10" s="65"/>
       <c r="E10" s="81"/>
@@ -3886,7 +3940,7 @@
       <c r="A11" s="76"/>
       <c r="B11" s="73"/>
       <c r="C11" s="64" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D11" s="65"/>
       <c r="E11" s="81"/>
@@ -3894,13 +3948,13 @@
     </row>
     <row r="12" customHeight="1" spans="1:6">
       <c r="A12" s="74" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B12" s="62" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C12" s="62" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D12" s="62"/>
       <c r="E12" s="62"/>
@@ -3912,7 +3966,7 @@
       <c r="A13" s="75"/>
       <c r="B13" s="62"/>
       <c r="C13" s="62" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D13" s="62"/>
       <c r="E13" s="62"/>
@@ -3922,7 +3976,7 @@
       <c r="A14" s="76"/>
       <c r="B14" s="62"/>
       <c r="C14" s="62" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D14" s="62"/>
       <c r="E14" s="62"/>
@@ -3930,13 +3984,13 @@
     </row>
     <row r="15" customHeight="1" spans="1:6">
       <c r="A15" s="74" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B15" s="69" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C15" s="64" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D15" s="65"/>
       <c r="E15" s="81"/>
@@ -3948,7 +4002,7 @@
       <c r="A16" s="75"/>
       <c r="B16" s="71"/>
       <c r="C16" s="64" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D16" s="65"/>
       <c r="E16" s="81"/>
@@ -3958,7 +4012,7 @@
       <c r="A17" s="75"/>
       <c r="B17" s="71"/>
       <c r="C17" s="64" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D17" s="65"/>
       <c r="E17" s="81"/>
@@ -3968,7 +4022,7 @@
       <c r="A18" s="76"/>
       <c r="B18" s="73"/>
       <c r="C18" s="64" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D18" s="65"/>
       <c r="E18" s="81"/>
@@ -3976,13 +4030,13 @@
     </row>
     <row r="19" customHeight="1" spans="1:6">
       <c r="A19" s="74" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B19" s="69" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D19" s="65"/>
       <c r="E19" s="81"/>
@@ -3994,7 +4048,7 @@
       <c r="A20" s="75"/>
       <c r="B20" s="71"/>
       <c r="C20" s="64" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D20" s="65"/>
       <c r="E20" s="81"/>
@@ -4004,7 +4058,7 @@
       <c r="A21" s="75"/>
       <c r="B21" s="71"/>
       <c r="C21" s="64" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D21" s="65"/>
       <c r="E21" s="81"/>
@@ -4014,7 +4068,7 @@
       <c r="A22" s="76"/>
       <c r="B22" s="73"/>
       <c r="C22" s="64" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D22" s="65"/>
       <c r="E22" s="81"/>
@@ -4022,13 +4076,13 @@
     </row>
     <row r="23" customHeight="1" spans="1:6">
       <c r="A23" s="74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B23" s="69" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C23" s="64" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D23" s="65"/>
       <c r="E23" s="81"/>
@@ -4040,7 +4094,7 @@
       <c r="A24" s="75"/>
       <c r="B24" s="71"/>
       <c r="C24" s="64" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D24" s="65"/>
       <c r="E24" s="81"/>
@@ -4050,7 +4104,7 @@
       <c r="A25" s="75"/>
       <c r="B25" s="71"/>
       <c r="C25" s="64" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D25" s="65"/>
       <c r="E25" s="81"/>
@@ -4060,7 +4114,7 @@
       <c r="A26" s="76"/>
       <c r="B26" s="73"/>
       <c r="C26" s="64" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D26" s="65"/>
       <c r="E26" s="81"/>
@@ -4068,7 +4122,7 @@
     </row>
     <row r="27" customHeight="1" spans="1:6">
       <c r="A27" s="77" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B27" s="78"/>
       <c r="C27" s="78"/>
@@ -4136,7 +4190,7 @@
   <dimension ref="B1:H27"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -4152,7 +4206,7 @@
   <sheetData>
     <row r="1" ht="45" customHeight="1" spans="2:7">
       <c r="B1" s="88" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C1" s="88"/>
       <c r="D1" s="88"/>
@@ -4162,7 +4216,7 @@
     </row>
     <row r="2" ht="45" customHeight="1" spans="2:7">
       <c r="B2" s="89" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C2" s="89"/>
       <c r="D2" s="89"/>
@@ -4282,11 +4336,11 @@
       <c r="F10" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="121" t="s">
+      <c r="G10" s="122" t="s">
         <v>26</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" ht="24.9" customHeight="1" spans="2:7">
@@ -4294,10 +4348,12 @@
         <v>14</v>
       </c>
       <c r="C11" s="98" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D11" s="92"/>
-      <c r="E11" s="95"/>
+      <c r="E11" s="115">
+        <v>10</v>
+      </c>
       <c r="F11" s="95"/>
       <c r="G11" s="92"/>
     </row>
@@ -4306,24 +4362,28 @@
         <v>27</v>
       </c>
       <c r="C12" s="98" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D12" s="92">
         <v>8</v>
       </c>
-      <c r="E12" s="95"/>
+      <c r="E12" s="115">
+        <v>8</v>
+      </c>
       <c r="F12" s="95"/>
       <c r="G12" s="92"/>
     </row>
     <row r="13" ht="24.9" customHeight="1" spans="2:7">
       <c r="B13" s="92" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C13" s="98" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D13" s="92"/>
-      <c r="E13" s="95"/>
+      <c r="E13" s="115">
+        <v>4</v>
+      </c>
       <c r="F13" s="95"/>
       <c r="G13" s="92"/>
     </row>
@@ -4332,10 +4392,12 @@
         <v>17</v>
       </c>
       <c r="C14" s="98" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D14" s="92"/>
-      <c r="E14" s="92"/>
+      <c r="E14" s="115">
+        <v>20</v>
+      </c>
       <c r="F14" s="92"/>
       <c r="G14" s="92"/>
     </row>
@@ -4344,10 +4406,12 @@
         <v>17</v>
       </c>
       <c r="C15" s="98" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D15" s="92"/>
-      <c r="E15" s="92"/>
+      <c r="E15" s="115">
+        <v>20</v>
+      </c>
       <c r="F15" s="92"/>
       <c r="G15" s="92"/>
     </row>
@@ -4356,11 +4420,13 @@
         <v>36</v>
       </c>
       <c r="C16" s="98" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D16" s="92"/>
-      <c r="E16" s="95"/>
-      <c r="F16" s="122"/>
+      <c r="E16" s="115">
+        <v>10</v>
+      </c>
+      <c r="F16" s="123"/>
       <c r="G16" s="92"/>
     </row>
     <row r="17" ht="24.9" customHeight="1" spans="2:7">
@@ -4368,10 +4434,12 @@
         <v>14</v>
       </c>
       <c r="C17" s="98" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D17" s="92"/>
-      <c r="E17" s="95"/>
+      <c r="E17" s="115">
+        <v>20</v>
+      </c>
       <c r="F17" s="95"/>
       <c r="G17" s="92"/>
     </row>
@@ -4380,10 +4448,10 @@
         <v>17</v>
       </c>
       <c r="C18" s="98" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D18" s="92"/>
-      <c r="E18" s="95"/>
+      <c r="E18" s="115"/>
       <c r="F18" s="95"/>
       <c r="G18" s="92"/>
     </row>
@@ -4392,10 +4460,10 @@
         <v>17</v>
       </c>
       <c r="C19" s="98" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D19" s="92"/>
-      <c r="E19" s="95"/>
+      <c r="E19" s="115"/>
       <c r="F19" s="95"/>
       <c r="G19" s="92"/>
     </row>
@@ -4404,12 +4472,14 @@
         <v>27</v>
       </c>
       <c r="C20" s="98" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D20" s="92">
         <v>2</v>
       </c>
-      <c r="E20" s="95"/>
+      <c r="E20" s="115">
+        <v>8</v>
+      </c>
       <c r="F20" s="95"/>
       <c r="G20" s="92"/>
     </row>
@@ -4417,11 +4487,13 @@
       <c r="B21" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="120" t="s">
-        <v>105</v>
+      <c r="C21" s="121" t="s">
+        <v>106</v>
       </c>
       <c r="D21" s="92"/>
-      <c r="E21" s="95"/>
+      <c r="E21" s="115">
+        <v>6</v>
+      </c>
       <c r="F21" s="95"/>
       <c r="G21" s="92"/>
     </row>
@@ -4451,14 +4523,14 @@
     <row r="25" ht="24.9" customHeight="1" spans="2:7">
       <c r="B25" s="92"/>
       <c r="C25" s="92" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D25" s="92"/>
       <c r="E25" s="95">
         <f>SUM(E12:E23,E11)</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="115">
+        <v>106</v>
+      </c>
+      <c r="F25" s="116">
         <f>SUM(F11:F23)</f>
         <v>0</v>
       </c>
@@ -4466,23 +4538,23 @@
     </row>
     <row r="26" ht="78" customHeight="1" spans="2:7">
       <c r="B26" s="99" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C26" s="100"/>
       <c r="D26" s="100"/>
       <c r="E26" s="100"/>
       <c r="F26" s="100"/>
-      <c r="G26" s="118"/>
+      <c r="G26" s="119"/>
     </row>
     <row r="27" ht="136.5" customHeight="1" spans="2:7">
       <c r="B27" s="101" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C27" s="102"/>
       <c r="D27" s="102"/>
       <c r="E27" s="102"/>
       <c r="F27" s="102"/>
-      <c r="G27" s="119"/>
+      <c r="G27" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -4520,7 +4592,7 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:6">
       <c r="A1" s="59" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
@@ -4530,30 +4602,30 @@
     </row>
     <row r="2" customHeight="1" spans="1:6">
       <c r="A2" s="61" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" s="62" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" s="63" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" s="62" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E2" s="61" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F2" s="80" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:6">
       <c r="A3" s="61" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B3" s="64" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C3" s="65"/>
       <c r="D3" s="65"/>
@@ -4562,29 +4634,29 @@
     </row>
     <row r="4" s="55" customFormat="1" customHeight="1" spans="1:6">
       <c r="A4" s="61" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" s="63" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C4" s="66" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D4" s="67"/>
       <c r="E4" s="82"/>
       <c r="F4" s="61" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="68" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B5" s="69" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D5" s="62"/>
       <c r="E5" s="62"/>
@@ -4596,7 +4668,7 @@
       <c r="A6" s="70"/>
       <c r="B6" s="71"/>
       <c r="C6" s="62" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D6" s="62"/>
       <c r="E6" s="62"/>
@@ -4606,7 +4678,7 @@
       <c r="A7" s="72"/>
       <c r="B7" s="73"/>
       <c r="C7" s="62" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D7" s="62"/>
       <c r="E7" s="62"/>
@@ -4614,13 +4686,13 @@
     </row>
     <row r="8" customHeight="1" spans="1:6">
       <c r="A8" s="74" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B8" s="69" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C8" s="64" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D8" s="65"/>
       <c r="E8" s="81"/>
@@ -4632,7 +4704,7 @@
       <c r="A9" s="75"/>
       <c r="B9" s="71"/>
       <c r="C9" s="64" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D9" s="65"/>
       <c r="E9" s="81"/>
@@ -4642,7 +4714,7 @@
       <c r="A10" s="75"/>
       <c r="B10" s="71"/>
       <c r="C10" s="64" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D10" s="65"/>
       <c r="E10" s="81"/>
@@ -4652,7 +4724,7 @@
       <c r="A11" s="76"/>
       <c r="B11" s="73"/>
       <c r="C11" s="64" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D11" s="65"/>
       <c r="E11" s="81"/>
@@ -4660,13 +4732,13 @@
     </row>
     <row r="12" customHeight="1" spans="1:6">
       <c r="A12" s="74" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B12" s="62" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C12" s="62" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D12" s="62"/>
       <c r="E12" s="62"/>
@@ -4678,7 +4750,7 @@
       <c r="A13" s="75"/>
       <c r="B13" s="62"/>
       <c r="C13" s="62" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D13" s="62"/>
       <c r="E13" s="62"/>
@@ -4688,7 +4760,7 @@
       <c r="A14" s="76"/>
       <c r="B14" s="62"/>
       <c r="C14" s="62" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D14" s="62"/>
       <c r="E14" s="62"/>
@@ -4696,13 +4768,13 @@
     </row>
     <row r="15" customHeight="1" spans="1:6">
       <c r="A15" s="74" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B15" s="69" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C15" s="64" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D15" s="65"/>
       <c r="E15" s="81"/>
@@ -4714,7 +4786,7 @@
       <c r="A16" s="75"/>
       <c r="B16" s="71"/>
       <c r="C16" s="64" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D16" s="65"/>
       <c r="E16" s="81"/>
@@ -4724,7 +4796,7 @@
       <c r="A17" s="75"/>
       <c r="B17" s="71"/>
       <c r="C17" s="64" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D17" s="65"/>
       <c r="E17" s="81"/>
@@ -4734,7 +4806,7 @@
       <c r="A18" s="76"/>
       <c r="B18" s="73"/>
       <c r="C18" s="64" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D18" s="65"/>
       <c r="E18" s="81"/>
@@ -4742,13 +4814,13 @@
     </row>
     <row r="19" customHeight="1" spans="1:6">
       <c r="A19" s="74" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B19" s="69" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D19" s="65"/>
       <c r="E19" s="81"/>
@@ -4760,7 +4832,7 @@
       <c r="A20" s="75"/>
       <c r="B20" s="71"/>
       <c r="C20" s="64" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D20" s="65"/>
       <c r="E20" s="81"/>
@@ -4770,7 +4842,7 @@
       <c r="A21" s="75"/>
       <c r="B21" s="71"/>
       <c r="C21" s="64" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D21" s="65"/>
       <c r="E21" s="81"/>
@@ -4780,7 +4852,7 @@
       <c r="A22" s="76"/>
       <c r="B22" s="73"/>
       <c r="C22" s="64" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D22" s="65"/>
       <c r="E22" s="81"/>
@@ -4788,13 +4860,13 @@
     </row>
     <row r="23" customHeight="1" spans="1:6">
       <c r="A23" s="74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B23" s="69" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C23" s="64" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D23" s="65"/>
       <c r="E23" s="81"/>
@@ -4806,7 +4878,7 @@
       <c r="A24" s="75"/>
       <c r="B24" s="71"/>
       <c r="C24" s="64" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D24" s="65"/>
       <c r="E24" s="81"/>
@@ -4816,7 +4888,7 @@
       <c r="A25" s="75"/>
       <c r="B25" s="71"/>
       <c r="C25" s="64" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D25" s="65"/>
       <c r="E25" s="81"/>
@@ -4826,7 +4898,7 @@
       <c r="A26" s="76"/>
       <c r="B26" s="73"/>
       <c r="C26" s="64" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D26" s="65"/>
       <c r="E26" s="81"/>
@@ -4834,7 +4906,7 @@
     </row>
     <row r="27" customHeight="1" spans="1:6">
       <c r="A27" s="77" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B27" s="78"/>
       <c r="C27" s="78"/>
@@ -4901,8 +4973,8 @@
   <sheetPr/>
   <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24.9" customHeight="1" outlineLevelCol="7"/>
@@ -4918,7 +4990,7 @@
   <sheetData>
     <row r="1" ht="45" customHeight="1" spans="2:8">
       <c r="B1" s="88" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C1" s="88"/>
       <c r="D1" s="88"/>
@@ -4929,7 +5001,7 @@
     </row>
     <row r="2" ht="45" customHeight="1" spans="2:8">
       <c r="B2" s="89" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C2" s="89"/>
       <c r="D2" s="89"/>
@@ -5067,14 +5139,16 @@
         <v>36</v>
       </c>
       <c r="C11" s="98" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D11" s="92">
         <v>2</v>
       </c>
-      <c r="E11" s="95"/>
-      <c r="F11" s="115"/>
-      <c r="G11" s="116"/>
+      <c r="E11" s="115">
+        <v>4</v>
+      </c>
+      <c r="F11" s="116"/>
+      <c r="G11" s="117"/>
       <c r="H11" s="92"/>
     </row>
     <row r="12" customHeight="1" spans="2:8">
@@ -5082,14 +5156,16 @@
         <v>30</v>
       </c>
       <c r="C12" s="98" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D12" s="92">
         <v>8</v>
       </c>
-      <c r="E12" s="95"/>
-      <c r="F12" s="115"/>
-      <c r="G12" s="116"/>
+      <c r="E12" s="115">
+        <v>10</v>
+      </c>
+      <c r="F12" s="116"/>
+      <c r="G12" s="117"/>
       <c r="H12" s="92"/>
     </row>
     <row r="13" customHeight="1" spans="2:8">
@@ -5097,14 +5173,16 @@
         <v>14</v>
       </c>
       <c r="C13" s="98" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D13" s="92">
         <v>8</v>
       </c>
-      <c r="E13" s="95"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="117"/>
+      <c r="E13" s="115">
+        <v>10</v>
+      </c>
+      <c r="F13" s="116"/>
+      <c r="G13" s="118"/>
       <c r="H13" s="92"/>
     </row>
     <row r="14" customHeight="1" spans="2:8">
@@ -5112,14 +5190,16 @@
         <v>27</v>
       </c>
       <c r="C14" s="98" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D14" s="92">
         <v>3</v>
       </c>
-      <c r="E14" s="92"/>
-      <c r="F14" s="115"/>
-      <c r="G14" s="117"/>
+      <c r="E14" s="115">
+        <v>6</v>
+      </c>
+      <c r="F14" s="116"/>
+      <c r="G14" s="118"/>
       <c r="H14" s="92"/>
     </row>
     <row r="15" customHeight="1" spans="2:8">
@@ -5127,14 +5207,16 @@
         <v>36</v>
       </c>
       <c r="C15" s="98" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D15" s="92">
         <v>2</v>
       </c>
-      <c r="E15" s="92"/>
-      <c r="F15" s="115"/>
-      <c r="G15" s="117"/>
+      <c r="E15" s="115">
+        <v>10</v>
+      </c>
+      <c r="F15" s="116"/>
+      <c r="G15" s="118"/>
       <c r="H15" s="92"/>
     </row>
     <row r="16" customHeight="1" spans="2:8">
@@ -5142,16 +5224,18 @@
         <v>14</v>
       </c>
       <c r="C16" s="98" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D16" s="92">
         <v>20</v>
       </c>
-      <c r="E16" s="92"/>
-      <c r="F16" s="115"/>
-      <c r="G16" s="117"/>
+      <c r="E16" s="115">
+        <v>20</v>
+      </c>
+      <c r="F16" s="116"/>
+      <c r="G16" s="118"/>
       <c r="H16" s="92" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="2:8">
@@ -5159,14 +5243,16 @@
         <v>17</v>
       </c>
       <c r="C17" s="98" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D17" s="92">
         <v>20</v>
       </c>
-      <c r="E17" s="92"/>
-      <c r="F17" s="115"/>
-      <c r="G17" s="117"/>
+      <c r="E17" s="115">
+        <v>20</v>
+      </c>
+      <c r="F17" s="116"/>
+      <c r="G17" s="118"/>
       <c r="H17" s="92"/>
     </row>
     <row r="18" customHeight="1" spans="2:8">
@@ -5174,14 +5260,16 @@
         <v>17</v>
       </c>
       <c r="C18" s="98" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D18" s="92">
         <v>20</v>
       </c>
-      <c r="E18" s="92"/>
-      <c r="F18" s="115"/>
-      <c r="G18" s="117"/>
+      <c r="E18" s="115">
+        <v>20</v>
+      </c>
+      <c r="F18" s="116"/>
+      <c r="G18" s="118"/>
       <c r="H18" s="92"/>
     </row>
     <row r="19" customHeight="1" spans="2:8">
@@ -5189,48 +5277,53 @@
         <v>27</v>
       </c>
       <c r="C19" s="98" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D19" s="92">
         <v>3</v>
       </c>
-      <c r="E19" s="95"/>
-      <c r="F19" s="115"/>
-      <c r="G19" s="117"/>
+      <c r="E19" s="115">
+        <v>6</v>
+      </c>
+      <c r="F19" s="116"/>
+      <c r="G19" s="118"/>
       <c r="H19" s="92"/>
     </row>
     <row r="20" customHeight="1" spans="2:8">
       <c r="B20" s="92"/>
       <c r="C20" s="92" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D20" s="92"/>
-      <c r="E20" s="95"/>
-      <c r="F20" s="115"/>
-      <c r="G20" s="116"/>
+      <c r="E20" s="95">
+        <f>SUM(E11:E19)</f>
+        <v>106</v>
+      </c>
+      <c r="F20" s="116"/>
+      <c r="G20" s="117"/>
       <c r="H20" s="92"/>
     </row>
     <row r="21" ht="79.05" customHeight="1" spans="2:8">
       <c r="B21" s="99" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C21" s="100"/>
       <c r="D21" s="100"/>
       <c r="E21" s="100"/>
       <c r="F21" s="100"/>
       <c r="G21" s="100"/>
-      <c r="H21" s="118"/>
+      <c r="H21" s="119"/>
     </row>
     <row r="22" ht="136.5" customHeight="1" spans="2:8">
       <c r="B22" s="101" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C22" s="102"/>
       <c r="D22" s="102"/>
       <c r="E22" s="102"/>
       <c r="F22" s="102"/>
       <c r="G22" s="102"/>
-      <c r="H22" s="119"/>
+      <c r="H22" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -5281,7 +5374,7 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:6">
       <c r="A1" s="59" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B1" s="60"/>
       <c r="C1" s="60"/>
@@ -5291,30 +5384,30 @@
     </row>
     <row r="2" customHeight="1" spans="1:6">
       <c r="A2" s="61" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" s="62" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C2" s="63" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" s="62" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E2" s="61" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F2" s="80" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:6">
       <c r="A3" s="61" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B3" s="64" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C3" s="65"/>
       <c r="D3" s="65"/>
@@ -5323,29 +5416,29 @@
     </row>
     <row r="4" s="55" customFormat="1" customHeight="1" spans="1:6">
       <c r="A4" s="61" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" s="63" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C4" s="66" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D4" s="67"/>
       <c r="E4" s="82"/>
       <c r="F4" s="61" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:6">
       <c r="A5" s="68" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B5" s="69" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D5" s="62"/>
       <c r="E5" s="62"/>
@@ -5357,7 +5450,7 @@
       <c r="A6" s="70"/>
       <c r="B6" s="71"/>
       <c r="C6" s="62" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D6" s="62"/>
       <c r="E6" s="62"/>
@@ -5367,7 +5460,7 @@
       <c r="A7" s="72"/>
       <c r="B7" s="73"/>
       <c r="C7" s="62" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D7" s="62"/>
       <c r="E7" s="62"/>
@@ -5375,13 +5468,13 @@
     </row>
     <row r="8" customHeight="1" spans="1:6">
       <c r="A8" s="74" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B8" s="69" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C8" s="64" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D8" s="65"/>
       <c r="E8" s="81"/>
@@ -5393,7 +5486,7 @@
       <c r="A9" s="75"/>
       <c r="B9" s="71"/>
       <c r="C9" s="64" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D9" s="65"/>
       <c r="E9" s="81"/>
@@ -5403,7 +5496,7 @@
       <c r="A10" s="75"/>
       <c r="B10" s="71"/>
       <c r="C10" s="64" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D10" s="65"/>
       <c r="E10" s="81"/>
@@ -5413,7 +5506,7 @@
       <c r="A11" s="76"/>
       <c r="B11" s="73"/>
       <c r="C11" s="64" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D11" s="65"/>
       <c r="E11" s="81"/>
@@ -5421,13 +5514,13 @@
     </row>
     <row r="12" customHeight="1" spans="1:6">
       <c r="A12" s="74" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B12" s="62" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C12" s="62" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D12" s="62"/>
       <c r="E12" s="62"/>
@@ -5439,7 +5532,7 @@
       <c r="A13" s="75"/>
       <c r="B13" s="62"/>
       <c r="C13" s="62" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D13" s="62"/>
       <c r="E13" s="62"/>
@@ -5449,7 +5542,7 @@
       <c r="A14" s="76"/>
       <c r="B14" s="62"/>
       <c r="C14" s="62" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D14" s="62"/>
       <c r="E14" s="62"/>
@@ -5457,13 +5550,13 @@
     </row>
     <row r="15" customHeight="1" spans="1:6">
       <c r="A15" s="74" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B15" s="69" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C15" s="64" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D15" s="65"/>
       <c r="E15" s="81"/>
@@ -5475,7 +5568,7 @@
       <c r="A16" s="75"/>
       <c r="B16" s="71"/>
       <c r="C16" s="64" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D16" s="65"/>
       <c r="E16" s="81"/>
@@ -5485,7 +5578,7 @@
       <c r="A17" s="75"/>
       <c r="B17" s="71"/>
       <c r="C17" s="64" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D17" s="65"/>
       <c r="E17" s="81"/>
@@ -5495,7 +5588,7 @@
       <c r="A18" s="76"/>
       <c r="B18" s="73"/>
       <c r="C18" s="64" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D18" s="65"/>
       <c r="E18" s="81"/>
@@ -5503,13 +5596,13 @@
     </row>
     <row r="19" customHeight="1" spans="1:6">
       <c r="A19" s="74" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B19" s="69" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D19" s="65"/>
       <c r="E19" s="81"/>
@@ -5521,7 +5614,7 @@
       <c r="A20" s="75"/>
       <c r="B20" s="71"/>
       <c r="C20" s="64" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D20" s="65"/>
       <c r="E20" s="81"/>
@@ -5531,7 +5624,7 @@
       <c r="A21" s="75"/>
       <c r="B21" s="71"/>
       <c r="C21" s="64" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D21" s="65"/>
       <c r="E21" s="81"/>
@@ -5541,7 +5634,7 @@
       <c r="A22" s="76"/>
       <c r="B22" s="73"/>
       <c r="C22" s="64" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D22" s="65"/>
       <c r="E22" s="81"/>
@@ -5549,13 +5642,13 @@
     </row>
     <row r="23" customHeight="1" spans="1:6">
       <c r="A23" s="74" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B23" s="69" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C23" s="64" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D23" s="65"/>
       <c r="E23" s="81"/>
@@ -5567,7 +5660,7 @@
       <c r="A24" s="75"/>
       <c r="B24" s="71"/>
       <c r="C24" s="64" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D24" s="65"/>
       <c r="E24" s="81"/>
@@ -5577,7 +5670,7 @@
       <c r="A25" s="75"/>
       <c r="B25" s="71"/>
       <c r="C25" s="64" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D25" s="65"/>
       <c r="E25" s="81"/>
@@ -5587,7 +5680,7 @@
       <c r="A26" s="76"/>
       <c r="B26" s="73"/>
       <c r="C26" s="64" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D26" s="65"/>
       <c r="E26" s="81"/>
@@ -5595,7 +5688,7 @@
     </row>
     <row r="27" ht="45" customHeight="1" spans="1:6">
       <c r="A27" s="77" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B27" s="78"/>
       <c r="C27" s="78"/>
@@ -5605,7 +5698,7 @@
     </row>
     <row r="29" customHeight="1" spans="1:1">
       <c r="A29" s="55" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -5688,7 +5781,7 @@
   <sheetData>
     <row r="1" ht="47.1" customHeight="1" spans="1:10">
       <c r="A1" s="23" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
@@ -5702,39 +5795,39 @@
     </row>
     <row r="2" ht="29.1" customHeight="1" spans="1:10">
       <c r="A2" s="24" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
       <c r="D2" s="25"/>
       <c r="E2" s="25" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H2" s="25"/>
       <c r="I2" s="25" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J2" s="45"/>
     </row>
     <row r="3" ht="27" customHeight="1" spans="1:10">
       <c r="A3" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
       <c r="D3" s="27"/>
       <c r="E3" s="27" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F3" s="27"/>
       <c r="G3" s="27" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H3" s="27"/>
       <c r="I3" s="46"/>
@@ -5742,7 +5835,7 @@
     </row>
     <row r="4" ht="14.25" customHeight="1" spans="1:10">
       <c r="A4" s="28" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
@@ -5756,11 +5849,11 @@
     </row>
     <row r="5" ht="14.25" customHeight="1" spans="1:10">
       <c r="A5" s="29" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="30" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D5" s="31"/>
       <c r="E5" s="31"/>
@@ -5786,7 +5879,7 @@
       <c r="A7" s="29"/>
       <c r="B7" s="29"/>
       <c r="C7" s="30" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D7" s="31"/>
       <c r="E7" s="31"/>
@@ -5810,11 +5903,11 @@
     </row>
     <row r="9" ht="14.25" customHeight="1" spans="1:10">
       <c r="A9" s="36" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B9" s="36"/>
       <c r="C9" s="30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="31"/>
@@ -5840,7 +5933,7 @@
       <c r="A11" s="36"/>
       <c r="B11" s="36"/>
       <c r="C11" s="37" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D11" s="38"/>
       <c r="E11" s="38"/>
@@ -5866,7 +5959,7 @@
       <c r="A13" s="36"/>
       <c r="B13" s="36"/>
       <c r="C13" s="37" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D13" s="38"/>
       <c r="E13" s="38"/>
@@ -5890,11 +5983,11 @@
     </row>
     <row r="15" ht="14.25" customHeight="1" spans="1:10">
       <c r="A15" s="36" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B15" s="36"/>
       <c r="C15" s="37" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D15" s="38"/>
       <c r="E15" s="38"/>
@@ -5920,7 +6013,7 @@
       <c r="A17" s="36"/>
       <c r="B17" s="36"/>
       <c r="C17" s="37" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D17" s="38"/>
       <c r="E17" s="38"/>
@@ -5944,11 +6037,11 @@
     </row>
     <row r="19" ht="14.25" customHeight="1" spans="1:10">
       <c r="A19" s="36" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B19" s="36"/>
       <c r="C19" s="37" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D19" s="38"/>
       <c r="E19" s="38"/>
@@ -5974,7 +6067,7 @@
       <c r="A21" s="36"/>
       <c r="B21" s="36"/>
       <c r="C21" s="37" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D21" s="38"/>
       <c r="E21" s="38"/>
@@ -5998,7 +6091,7 @@
     </row>
     <row r="23" ht="14.25" customHeight="1" spans="1:10">
       <c r="A23" s="41" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B23" s="41"/>
       <c r="C23" s="41"/>
@@ -6012,10 +6105,10 @@
     </row>
     <row r="24" ht="14.25" customHeight="1" spans="1:10">
       <c r="A24" s="36" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B24" s="37" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C24" s="38"/>
       <c r="D24" s="38"/>
@@ -6040,10 +6133,10 @@
     </row>
     <row r="26" ht="14.25" customHeight="1" spans="1:10">
       <c r="A26" s="36" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C26" s="38"/>
       <c r="D26" s="38"/>
@@ -6068,10 +6161,10 @@
     </row>
     <row r="28" ht="14.25" customHeight="1" spans="1:10">
       <c r="A28" s="36" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C28" s="38"/>
       <c r="D28" s="38"/>
@@ -6096,10 +6189,10 @@
     </row>
     <row r="30" ht="14.25" customHeight="1" spans="1:10">
       <c r="A30" s="44" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B30" s="37" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C30" s="38"/>
       <c r="D30" s="38"/>
@@ -6191,36 +6284,36 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:5">
@@ -6247,13 +6340,13 @@
     <row r="6" ht="75" customHeight="1" spans="1:5">
       <c r="A6" s="1"/>
       <c r="B6" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E6" s="17"/>
     </row>
@@ -6263,13 +6356,13 @@
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:5">
@@ -6277,78 +6370,78 @@
         <v>20</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:5">
       <c r="A9" s="12"/>
       <c r="B9" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E9" s="20"/>
     </row>
     <row r="10" customHeight="1" spans="1:5">
       <c r="A10" s="12"/>
       <c r="B10" s="8" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E10" s="20"/>
     </row>
     <row r="11" ht="60" customHeight="1" spans="1:5">
       <c r="A11" s="13"/>
       <c r="B11" s="8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E11" s="21"/>
     </row>
     <row r="12" customHeight="1" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:5">
       <c r="A13" s="1"/>
       <c r="B13" s="8" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -6357,7 +6450,7 @@
     <row r="14" ht="11" customHeight="1" spans="1:5">
       <c r="A14" s="1"/>
       <c r="B14" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -6365,72 +6458,72 @@
     </row>
     <row r="15" customHeight="1" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" ht="66" customHeight="1" spans="1:5">
       <c r="A16" s="1"/>
       <c r="B16" s="8" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E16" s="17"/>
     </row>
     <row r="17" customHeight="1" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E17" s="8"/>
     </row>
     <row r="18" customHeight="1" spans="1:5">
       <c r="A18" s="1"/>
       <c r="B18" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E18" s="8"/>
     </row>
     <row r="19" ht="60" customHeight="1" spans="1:5">
       <c r="A19" s="1"/>
       <c r="B19" s="8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E19" s="8"/>
     </row>
     <row r="20" ht="261" customHeight="1" spans="1:5">
       <c r="A20" s="14" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -6439,7 +6532,7 @@
     </row>
     <row r="22" ht="39" customHeight="1" spans="1:1">
       <c r="A22" s="16" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>